<commit_message>
Version 1.1, 1 Abril 2020 (actualización de modelo)
</commit_message>
<xml_diff>
--- a/temp/_Transelectric.xlsx
+++ b/temp/_Transelectric.xlsx
@@ -49,10 +49,13 @@
     <t>UTR_S_IDELFO_RP5</t>
   </si>
   <si>
+    <t>UTR_MACAS_IEC8705101</t>
+  </si>
+  <si>
     <t>UTR_YANACOCH_IEC8705101</t>
   </si>
   <si>
-    <t>UTR_MACAS_IEC8705101</t>
+    <t>UTR_LIMON_IEC8705101</t>
   </si>
   <si>
     <t>UTR_N_BABAHO_IEC8705101</t>
@@ -67,166 +70,166 @@
     <t>UTR_POSORJA_RP5</t>
   </si>
   <si>
+    <t>UTR_E_GUAYAQ_DNP</t>
+  </si>
+  <si>
     <t>UTR_QUININDE_IEC8705101</t>
   </si>
   <si>
-    <t>UTR_E_GUAYAQ_DNP</t>
+    <t>UTR_D_CERRIT_RP5</t>
+  </si>
+  <si>
+    <t>UTR_TOTORAS_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_ESMERALD_IEC8705104</t>
+  </si>
+  <si>
+    <t>UTR_ESCLUSAS_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_TRINITAR_RP5</t>
+  </si>
+  <si>
+    <t>UTR_IBARRA_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_ZHORAY_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_S_ROSA_IEC8705101</t>
   </si>
   <si>
     <t>UTR_RIOBAMBA_RP5</t>
   </si>
   <si>
-    <t>UTR_ZHORAY_IEC8705101</t>
+    <t>UTR_S_ELENA_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_MACHALA_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_JIVINO_IEC8705104</t>
+  </si>
+  <si>
+    <t>UTR_PASCUALE_IEC8705101</t>
   </si>
   <si>
     <t>UTR_BANOS_IEC8705101</t>
   </si>
   <si>
-    <t>UTR_IBARRA_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_ESCLUSAS_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_ESMERALD_IEC8705104</t>
-  </si>
-  <si>
-    <t>UTR_TRINITAR_RP5</t>
-  </si>
-  <si>
-    <t>UTR_S_ROSA_IEC8705101</t>
+    <t>UTR_TADAY_IEC8705104</t>
+  </si>
+  <si>
+    <t>UTR_SININCAY_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_INGA_500_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_MENDEZ_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_S_GREGOR_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_INGA_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_POLICENT_RP5</t>
+  </si>
+  <si>
+    <t>UTR_MULALO_RP5</t>
+  </si>
+  <si>
+    <t>UTR_TGMA_COR_RP5</t>
+  </si>
+  <si>
+    <t>UTR_S_ELENA_RP5</t>
+  </si>
+  <si>
+    <t>UTR_SALITRAL_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_CHORRILL_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_POMASQUI_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_QUEVEDO_RP5</t>
+  </si>
+  <si>
+    <t>UTR_TOTORAS_RP5</t>
+  </si>
+  <si>
+    <t>UTR_PORTOVIE_RP5</t>
+  </si>
+  <si>
+    <t>UTR_AMBATO_RP5</t>
+  </si>
+  <si>
+    <t>UTR_BOMBOIZA_IEC8705104</t>
+  </si>
+  <si>
+    <t>UTR_GUALACEO_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_BABA_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_POMASQUI_RP5</t>
+  </si>
+  <si>
+    <t>UTR_TOPO_IEC8705101</t>
+  </si>
+  <si>
+    <t>UTR_LOJA_RP5</t>
+  </si>
+  <si>
+    <t>UTR_LORETO_IEC8705104</t>
+  </si>
+  <si>
+    <t>UTR_MOLINO_RP5</t>
+  </si>
+  <si>
+    <t>UTR_CHONE_RP5</t>
+  </si>
+  <si>
+    <t>UTR_CUENCA_RP5</t>
   </si>
   <si>
     <t>UTR_CHONGON_IEC8705101</t>
   </si>
   <si>
-    <t>UTR_GUALACEO_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_INGA_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_MACHALA_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_JIVINO_IEC8705104</t>
-  </si>
-  <si>
-    <t>UTR_TOTORAS_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_PASCUALE_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_QUEVEDO_RP5</t>
-  </si>
-  <si>
-    <t>UTR_LIMON_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_S_ELENA_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_BABA_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_D_CERRIT_RP5</t>
-  </si>
-  <si>
-    <t>UTR_TOTORAS_RP5</t>
-  </si>
-  <si>
-    <t>UTR_MENDEZ_IEC8705101</t>
-  </si>
-  <si>
     <t>UTR_TULCAN_RP5</t>
   </si>
   <si>
-    <t>UTR_AMBATO_RP5</t>
-  </si>
-  <si>
-    <t>UTR_TOPO_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_S_GREGOR_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_LORETO_IEC8705104</t>
-  </si>
-  <si>
-    <t>UTR_TADAY_IEC8705104</t>
-  </si>
-  <si>
-    <t>UTR_SININCAY_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_LOJA_RP5</t>
-  </si>
-  <si>
     <t>UTR_CARAGUAY_IEC8705101</t>
   </si>
   <si>
+    <t>UTR_S_RAFAEL_IEC8705101</t>
+  </si>
+  <si>
     <t>UTR_N_PROSPE_IEC8705101</t>
   </si>
   <si>
-    <t>UTR_MULALO_RP5</t>
-  </si>
-  <si>
-    <t>UTR_S_RAFAEL_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_PORTOVIE_RP5</t>
-  </si>
-  <si>
-    <t>UTR_CHONE_RP5</t>
-  </si>
-  <si>
-    <t>UTR_TGMA_COR_RP5</t>
-  </si>
-  <si>
-    <t>UTR_SALITRAL_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_INGA_500_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_S_ELENA_RP5</t>
-  </si>
-  <si>
-    <t>UTR_POLICENT_RP5</t>
+    <t>UTR_TISALEO_IEC8705104</t>
   </si>
   <si>
     <t>UTR_MILAGRO_IEC8705101</t>
   </si>
   <si>
-    <t>UTR_MOLINO_RP5</t>
-  </si>
-  <si>
-    <t>UTR_BOMBOIZA_IEC8705104</t>
-  </si>
-  <si>
-    <t>UTR_POMASQUI_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_CHORRILL_IEC8705101</t>
-  </si>
-  <si>
-    <t>UTR_TISALEO_IEC8705104</t>
-  </si>
-  <si>
-    <t>UTR_CUENCA_RP5</t>
-  </si>
-  <si>
-    <t>UTR_POMASQUI_RP5</t>
-  </si>
-  <si>
     <t>S. IDELFONSO</t>
   </si>
   <si>
+    <t>MACAS</t>
+  </si>
+  <si>
     <t>YANACOCH</t>
   </si>
   <si>
-    <t>MACAS</t>
+    <t>LIMON</t>
   </si>
   <si>
     <t>N_BABAHO</t>
@@ -241,145 +244,142 @@
     <t>POSORJA</t>
   </si>
   <si>
+    <t>E_GUAYAQ_DNP</t>
+  </si>
+  <si>
     <t>QUININDE</t>
   </si>
   <si>
-    <t>E_GUAYAQ_DNP</t>
+    <t>D_CERRIT</t>
+  </si>
+  <si>
+    <t>TOTORAS</t>
+  </si>
+  <si>
+    <t>ESCLUSAS</t>
+  </si>
+  <si>
+    <t>TRINITAR</t>
+  </si>
+  <si>
+    <t>IBARRA</t>
+  </si>
+  <si>
+    <t>ZHORAY</t>
+  </si>
+  <si>
+    <t>S_ROSA</t>
   </si>
   <si>
     <t>RIOBAMBA</t>
   </si>
   <si>
-    <t>ZHORAY</t>
+    <t>S_ELENA</t>
+  </si>
+  <si>
+    <t>MACHALA</t>
+  </si>
+  <si>
+    <t>JIVINO</t>
+  </si>
+  <si>
+    <t>PASCUALE</t>
   </si>
   <si>
     <t>BAÑOS</t>
   </si>
   <si>
-    <t>IBARRA</t>
-  </si>
-  <si>
-    <t>ESCLUSAS</t>
-  </si>
-  <si>
-    <t>TRINITAR</t>
-  </si>
-  <si>
-    <t>S_ROSA</t>
+    <t>TADAY</t>
+  </si>
+  <si>
+    <t>SININCAY</t>
+  </si>
+  <si>
+    <t>INGA</t>
+  </si>
+  <si>
+    <t>MENDEZ</t>
+  </si>
+  <si>
+    <t>S_GREGOR</t>
+  </si>
+  <si>
+    <t>POLICENT</t>
+  </si>
+  <si>
+    <t>MULALO</t>
+  </si>
+  <si>
+    <t>TGMA_COR</t>
+  </si>
+  <si>
+    <t>SALITRAL</t>
+  </si>
+  <si>
+    <t>CHORRILL</t>
+  </si>
+  <si>
+    <t>POMASQUI</t>
+  </si>
+  <si>
+    <t>QUEVEDO</t>
+  </si>
+  <si>
+    <t>PORTOVIE</t>
+  </si>
+  <si>
+    <t>AMBATO</t>
+  </si>
+  <si>
+    <t>BOMBOIZA</t>
+  </si>
+  <si>
+    <t>GUALACEO</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>TOPO</t>
+  </si>
+  <si>
+    <t>LOJA</t>
+  </si>
+  <si>
+    <t>LORETO</t>
+  </si>
+  <si>
+    <t>MOLINO</t>
+  </si>
+  <si>
+    <t>CHONE</t>
+  </si>
+  <si>
+    <t>CUENCA</t>
   </si>
   <si>
     <t>CHONGON</t>
   </si>
   <si>
-    <t>GUALACEO</t>
-  </si>
-  <si>
-    <t>INGA</t>
-  </si>
-  <si>
-    <t>MACHALA</t>
-  </si>
-  <si>
-    <t>JIVINO</t>
-  </si>
-  <si>
-    <t>TOTORAS</t>
-  </si>
-  <si>
-    <t>PASCUALE</t>
-  </si>
-  <si>
-    <t>QUEVEDO</t>
-  </si>
-  <si>
-    <t>LIMON</t>
-  </si>
-  <si>
-    <t>S_ELENA</t>
-  </si>
-  <si>
-    <t>BABA</t>
-  </si>
-  <si>
-    <t>D_CERRIT</t>
-  </si>
-  <si>
-    <t>MENDEZ</t>
-  </si>
-  <si>
     <t>TULCAN</t>
   </si>
   <si>
-    <t>AMBATO</t>
-  </si>
-  <si>
-    <t>TOPO</t>
-  </si>
-  <si>
-    <t>S_GREGOR</t>
-  </si>
-  <si>
-    <t>LORETO</t>
-  </si>
-  <si>
-    <t>TADAY</t>
-  </si>
-  <si>
-    <t>SININCAY</t>
-  </si>
-  <si>
-    <t>LOJA</t>
-  </si>
-  <si>
     <t>CARAGUAY</t>
   </si>
   <si>
+    <t>S_RAFAEL</t>
+  </si>
+  <si>
     <t>N_PROSPE</t>
   </si>
   <si>
-    <t>MULALO</t>
-  </si>
-  <si>
-    <t>S_RAFAEL</t>
-  </si>
-  <si>
-    <t>PORTOVIE</t>
-  </si>
-  <si>
-    <t>CHONE</t>
-  </si>
-  <si>
-    <t>TGMA_COR</t>
-  </si>
-  <si>
-    <t>SALITRAL</t>
-  </si>
-  <si>
-    <t>POLICENT</t>
+    <t>TISALEO</t>
   </si>
   <si>
     <t>MILAGRO</t>
   </si>
   <si>
-    <t>MOLINO</t>
-  </si>
-  <si>
-    <t>BOMBOIZA</t>
-  </si>
-  <si>
-    <t>POMASQUI</t>
-  </si>
-  <si>
-    <t>CHORRILL</t>
-  </si>
-  <si>
-    <t>TISALEO</t>
-  </si>
-  <si>
-    <t>CUENCA</t>
-  </si>
-  <si>
-    <t>2020-01-01 00:00:00 @ 2020-01-31 00:00:00</t>
+    <t>2020-03-01 00:00:00 @ 2020-03-06 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -783,16 +783,16 @@
         <v>68</v>
       </c>
       <c r="C2">
-        <v>568053.2666666666</v>
+        <v>71975.16666666667</v>
       </c>
       <c r="D2">
         <v>16</v>
       </c>
       <c r="E2">
-        <v>7696.67</v>
+        <v>2701.55</v>
       </c>
       <c r="F2">
-        <v>17.82</v>
+        <v>37.52</v>
       </c>
       <c r="G2">
         <v>0.007889546351084813</v>
@@ -801,7 +801,7 @@
         <v>121</v>
       </c>
       <c r="I2">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -812,25 +812,25 @@
         <v>69</v>
       </c>
       <c r="C3">
-        <v>269601.1456586202</v>
+        <v>33871.66541773478</v>
       </c>
       <c r="D3">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="E3">
-        <v>35711.08</v>
+        <v>5207.55</v>
       </c>
       <c r="F3">
-        <v>82.66</v>
+        <v>72.33</v>
       </c>
       <c r="G3">
-        <v>0.01775147928994083</v>
+        <v>0.008382642998027613</v>
       </c>
       <c r="H3" t="s">
         <v>121</v>
       </c>
       <c r="I3">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -841,25 +841,25 @@
         <v>70</v>
       </c>
       <c r="C4">
-        <v>111849.6790590922</v>
+        <v>52605.85</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E4">
-        <v>36620.61</v>
+        <v>5738.73</v>
       </c>
       <c r="F4">
-        <v>84.77</v>
+        <v>79.7</v>
       </c>
       <c r="G4">
-        <v>0.008382642998027613</v>
+        <v>0.01775147928994083</v>
       </c>
       <c r="H4" t="s">
         <v>121</v>
       </c>
       <c r="I4">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -870,25 +870,25 @@
         <v>71</v>
       </c>
       <c r="C5">
-        <v>177186.7578796387</v>
+        <v>18749.42561772664</v>
       </c>
       <c r="D5">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E5">
-        <v>37484.3</v>
+        <v>6213.19</v>
       </c>
       <c r="F5">
-        <v>86.77</v>
+        <v>86.29000000000001</v>
       </c>
       <c r="G5">
-        <v>0.01528599605522682</v>
+        <v>0.009368836291913214</v>
       </c>
       <c r="H5" t="s">
         <v>121</v>
       </c>
       <c r="I5">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -899,25 +899,25 @@
         <v>72</v>
       </c>
       <c r="C6">
-        <v>107670.2293525696</v>
+        <v>28800</v>
       </c>
       <c r="D6">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>38518.69</v>
+        <v>6270.97</v>
       </c>
       <c r="F6">
-        <v>89.16</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="G6">
-        <v>0.01134122287968442</v>
+        <v>0.01528599605522682</v>
       </c>
       <c r="H6" t="s">
         <v>121</v>
       </c>
       <c r="I6">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -928,16 +928,16 @@
         <v>73</v>
       </c>
       <c r="C7">
-        <v>86400</v>
+        <v>14542.8</v>
       </c>
       <c r="D7">
         <v>23</v>
       </c>
       <c r="E7">
-        <v>39443.48</v>
+        <v>6567.7</v>
       </c>
       <c r="F7">
-        <v>91.3</v>
+        <v>91.22</v>
       </c>
       <c r="G7">
         <v>0.01134122287968442</v>
@@ -946,7 +946,7 @@
         <v>121</v>
       </c>
       <c r="I7">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -957,25 +957,25 @@
         <v>74</v>
       </c>
       <c r="C8">
-        <v>93678.23333333334</v>
+        <v>14400</v>
       </c>
       <c r="D8">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8">
-        <v>39596.99</v>
+        <v>6573.91</v>
       </c>
       <c r="F8">
-        <v>91.66</v>
+        <v>91.3</v>
       </c>
       <c r="G8">
-        <v>0.01282051282051282</v>
+        <v>0.01134122287968442</v>
       </c>
       <c r="H8" t="s">
         <v>121</v>
       </c>
       <c r="I8">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -986,25 +986,25 @@
         <v>75</v>
       </c>
       <c r="C9">
-        <v>56369.85632019042</v>
+        <v>14400</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>39676.88</v>
+        <v>6646.15</v>
       </c>
       <c r="F9">
-        <v>91.84</v>
+        <v>92.31</v>
       </c>
       <c r="G9">
-        <v>0.007889546351084813</v>
+        <v>0.01282051282051282</v>
       </c>
       <c r="H9" t="s">
         <v>121</v>
       </c>
       <c r="I9">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1015,16 +1015,16 @@
         <v>76</v>
       </c>
       <c r="C10">
-        <v>323030.6592168172</v>
+        <v>52543.45</v>
       </c>
       <c r="D10">
         <v>109</v>
       </c>
       <c r="E10">
-        <v>40236.42</v>
+        <v>6717.95</v>
       </c>
       <c r="F10">
-        <v>93.14</v>
+        <v>93.3</v>
       </c>
       <c r="G10">
         <v>0.05374753451676528</v>
@@ -1033,7 +1033,7 @@
         <v>121</v>
       </c>
       <c r="I10">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1044,25 +1044,25 @@
         <v>77</v>
       </c>
       <c r="C11">
-        <v>88366.83333333334</v>
+        <v>7200</v>
       </c>
       <c r="D11">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <v>40934.18</v>
+        <v>6750</v>
       </c>
       <c r="F11">
-        <v>94.76000000000001</v>
+        <v>93.75</v>
       </c>
       <c r="G11">
-        <v>0.01923076923076923</v>
+        <v>0.007889546351084813</v>
       </c>
       <c r="H11" t="s">
         <v>121</v>
       </c>
       <c r="I11">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1073,25 +1073,25 @@
         <v>78</v>
       </c>
       <c r="C12">
-        <v>59178.05030110677</v>
+        <v>7073.933333333333</v>
       </c>
       <c r="D12">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E12">
-        <v>41086.5</v>
+        <v>6878.46</v>
       </c>
       <c r="F12">
-        <v>95.11</v>
+        <v>95.53</v>
       </c>
       <c r="G12">
-        <v>0.01380670611439842</v>
+        <v>0.01084812623274162</v>
       </c>
       <c r="H12" t="s">
         <v>121</v>
       </c>
       <c r="I12">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1102,25 +1102,25 @@
         <v>79</v>
       </c>
       <c r="C13">
-        <v>69456.01007003784</v>
+        <v>3102.709083302816</v>
       </c>
       <c r="D13">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E13">
-        <v>41322.81</v>
+        <v>6889.73</v>
       </c>
       <c r="F13">
-        <v>95.65000000000001</v>
+        <v>95.69</v>
       </c>
       <c r="G13">
-        <v>0.01824457593688363</v>
+        <v>0.004930966469428008</v>
       </c>
       <c r="H13" t="s">
         <v>121</v>
       </c>
       <c r="I13">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1128,19 +1128,19 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C14">
-        <v>88708.30223541259</v>
+        <v>14400</v>
       </c>
       <c r="D14">
         <v>50</v>
       </c>
       <c r="E14">
-        <v>41425.83</v>
+        <v>6912</v>
       </c>
       <c r="F14">
-        <v>95.89</v>
+        <v>96</v>
       </c>
       <c r="G14">
         <v>0.02465483234714004</v>
@@ -1149,7 +1149,7 @@
         <v>121</v>
       </c>
       <c r="I14">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1157,19 +1157,19 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15">
-        <v>86750.72017033896</v>
+        <v>14400</v>
       </c>
       <c r="D15">
         <v>50</v>
       </c>
       <c r="E15">
-        <v>41464.99</v>
+        <v>6912</v>
       </c>
       <c r="F15">
-        <v>95.98</v>
+        <v>96</v>
       </c>
       <c r="G15">
         <v>0.02465483234714004</v>
@@ -1178,7 +1178,7 @@
         <v>121</v>
       </c>
       <c r="I15">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1186,16 +1186,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C16">
-        <v>86500.38333333333</v>
+        <v>14400</v>
       </c>
       <c r="D16">
         <v>50</v>
       </c>
       <c r="E16">
-        <v>41469.99</v>
+        <v>6912</v>
       </c>
       <c r="F16">
         <v>96</v>
@@ -1207,7 +1207,7 @@
         <v>121</v>
       </c>
       <c r="I16">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1218,16 +1218,16 @@
         <v>82</v>
       </c>
       <c r="C17">
-        <v>86196.71666666667</v>
+        <v>14400</v>
       </c>
       <c r="D17">
         <v>50</v>
       </c>
       <c r="E17">
-        <v>41476.07</v>
+        <v>6912</v>
       </c>
       <c r="F17">
-        <v>96.01000000000001</v>
+        <v>96</v>
       </c>
       <c r="G17">
         <v>0.02465483234714004</v>
@@ -1236,7 +1236,7 @@
         <v>121</v>
       </c>
       <c r="I17">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1247,25 +1247,25 @@
         <v>83</v>
       </c>
       <c r="C18">
-        <v>87990.01238810224</v>
+        <v>7218.784350840251</v>
       </c>
       <c r="D18">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="E18">
-        <v>41924.78</v>
+        <v>6942.19</v>
       </c>
       <c r="F18">
-        <v>97.05</v>
+        <v>96.42</v>
       </c>
       <c r="G18">
-        <v>0.03402366863905325</v>
+        <v>0.01380670611439842</v>
       </c>
       <c r="H18" t="s">
         <v>121</v>
       </c>
       <c r="I18">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1276,25 +1276,25 @@
         <v>84</v>
       </c>
       <c r="C19">
-        <v>29050.71666666667</v>
+        <v>14396.99705022176</v>
       </c>
       <c r="D19">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="E19">
-        <v>42231.64</v>
+        <v>6991.35</v>
       </c>
       <c r="F19">
-        <v>97.76000000000001</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="G19">
-        <v>0.01479289940828402</v>
+        <v>0.03402366863905325</v>
       </c>
       <c r="H19" t="s">
         <v>121</v>
       </c>
       <c r="I19">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1305,25 +1305,25 @@
         <v>85</v>
       </c>
       <c r="C20">
-        <v>12618.04108632406</v>
+        <v>7200</v>
       </c>
       <c r="D20">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="E20">
-        <v>42298.71</v>
+        <v>7015.38</v>
       </c>
       <c r="F20">
-        <v>97.91</v>
+        <v>97.44</v>
       </c>
       <c r="G20">
-        <v>0.006903353057199211</v>
+        <v>0.01923076923076923</v>
       </c>
       <c r="H20" t="s">
         <v>121</v>
       </c>
       <c r="I20">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1334,25 +1334,25 @@
         <v>86</v>
       </c>
       <c r="C21">
-        <v>49550.01666666667</v>
+        <v>414.4513168334961</v>
       </c>
       <c r="D21">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>42413.49</v>
+        <v>7061.85</v>
       </c>
       <c r="F21">
-        <v>98.18000000000001</v>
+        <v>98.08</v>
       </c>
       <c r="G21">
-        <v>0.03106508875739645</v>
+        <v>0.001479289940828402</v>
       </c>
       <c r="H21" t="s">
         <v>121</v>
       </c>
       <c r="I21">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1363,16 +1363,16 @@
         <v>87</v>
       </c>
       <c r="C22">
-        <v>48159.80970815023</v>
+        <v>7847.819237518311</v>
       </c>
       <c r="D22">
         <v>67</v>
       </c>
       <c r="E22">
-        <v>42481.2</v>
+        <v>7082.87</v>
       </c>
       <c r="F22">
-        <v>98.34</v>
+        <v>98.37</v>
       </c>
       <c r="G22">
         <v>0.03303747534516766</v>
@@ -1381,7 +1381,7 @@
         <v>121</v>
       </c>
       <c r="I22">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1392,13 +1392,13 @@
         <v>88</v>
       </c>
       <c r="C23">
-        <v>43200</v>
+        <v>7200</v>
       </c>
       <c r="D23">
         <v>63</v>
       </c>
       <c r="E23">
-        <v>42514.29</v>
+        <v>7085.71</v>
       </c>
       <c r="F23">
         <v>98.41</v>
@@ -1410,7 +1410,7 @@
         <v>121</v>
       </c>
       <c r="I23">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1421,25 +1421,25 @@
         <v>89</v>
       </c>
       <c r="C24">
-        <v>6306.18848470052</v>
+        <v>7906.516250356039</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="E24">
-        <v>42569.38</v>
+        <v>7103.58</v>
       </c>
       <c r="F24">
-        <v>98.54000000000001</v>
+        <v>98.66</v>
       </c>
       <c r="G24">
-        <v>0.004930966469428008</v>
+        <v>0.04043392504930966</v>
       </c>
       <c r="H24" t="s">
         <v>121</v>
       </c>
       <c r="I24">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1450,25 +1450,25 @@
         <v>90</v>
       </c>
       <c r="C25">
-        <v>44218.78471781413</v>
+        <v>1027.881367238363</v>
       </c>
       <c r="D25">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E25">
-        <v>42660.75</v>
+        <v>7172.22</v>
       </c>
       <c r="F25">
-        <v>98.75</v>
+        <v>99.61</v>
       </c>
       <c r="G25">
-        <v>0.04043392504930966</v>
+        <v>0.01824457593688363</v>
       </c>
       <c r="H25" t="s">
         <v>121</v>
       </c>
       <c r="I25">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1479,25 +1479,25 @@
         <v>91</v>
       </c>
       <c r="C26">
-        <v>22288.78333333333</v>
+        <v>238.3962003072103</v>
       </c>
       <c r="D26">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E26">
-        <v>42704.69</v>
+        <v>7190.07</v>
       </c>
       <c r="F26">
-        <v>98.84999999999999</v>
+        <v>99.86</v>
       </c>
       <c r="G26">
-        <v>0.02218934911242603</v>
+        <v>0.01183431952662722</v>
       </c>
       <c r="H26" t="s">
         <v>121</v>
       </c>
       <c r="I26">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1508,25 +1508,25 @@
         <v>92</v>
       </c>
       <c r="C27">
-        <v>9082.804456075033</v>
+        <v>238.3962003072103</v>
       </c>
       <c r="D27">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E27">
-        <v>42721.96</v>
+        <v>7190.07</v>
       </c>
       <c r="F27">
-        <v>98.89</v>
+        <v>99.86</v>
       </c>
       <c r="G27">
-        <v>0.009368836291913214</v>
+        <v>0.01183431952662722</v>
       </c>
       <c r="H27" t="s">
         <v>121</v>
       </c>
       <c r="I27">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1537,25 +1537,25 @@
         <v>93</v>
       </c>
       <c r="C28">
-        <v>1061.426634470622</v>
+        <v>131.4</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E28">
-        <v>42846.19</v>
+        <v>7196.54</v>
       </c>
       <c r="F28">
-        <v>99.18000000000001</v>
+        <v>99.95</v>
       </c>
       <c r="G28">
-        <v>0.001479289940828402</v>
+        <v>0.01873767258382643</v>
       </c>
       <c r="H28" t="s">
         <v>121</v>
       </c>
       <c r="I28">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1566,25 +1566,25 @@
         <v>94</v>
       </c>
       <c r="C29">
-        <v>1319.075833892822</v>
+        <v>33.4017827351888</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E29">
-        <v>43068.09</v>
+        <v>7198.04</v>
       </c>
       <c r="F29">
-        <v>99.69</v>
+        <v>99.97</v>
       </c>
       <c r="G29">
-        <v>0.004930966469428008</v>
+        <v>0.008382642998027613</v>
       </c>
       <c r="H29" t="s">
         <v>121</v>
       </c>
       <c r="I29">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1595,25 +1595,25 @@
         <v>95</v>
       </c>
       <c r="C30">
-        <v>2569.283333333333</v>
+        <v>17.05635248819987</v>
       </c>
       <c r="D30">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E30">
-        <v>43083.21</v>
+        <v>7199.15</v>
       </c>
       <c r="F30">
-        <v>99.73</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="G30">
-        <v>0.01084812623274162</v>
+        <v>0.009861932938856016</v>
       </c>
       <c r="H30" t="s">
         <v>121</v>
       </c>
       <c r="I30">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1621,28 +1621,28 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C31">
-        <v>2454.866666666666</v>
+        <v>51.05</v>
       </c>
       <c r="D31">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E31">
-        <v>43145.45</v>
+        <v>7199.19</v>
       </c>
       <c r="F31">
-        <v>99.87</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="G31">
-        <v>0.02218934911242603</v>
+        <v>0.03106508875739645</v>
       </c>
       <c r="H31" t="s">
         <v>121</v>
       </c>
       <c r="I31">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1653,25 +1653,25 @@
         <v>96</v>
       </c>
       <c r="C32">
-        <v>919.5370152791342</v>
+        <v>14.05</v>
       </c>
       <c r="D32">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E32">
-        <v>43145.91</v>
+        <v>7199.48</v>
       </c>
       <c r="F32">
-        <v>99.87</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="G32">
-        <v>0.008382642998027613</v>
+        <v>0.01331360946745562</v>
       </c>
       <c r="H32" t="s">
         <v>121</v>
       </c>
       <c r="I32">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1682,25 +1682,25 @@
         <v>97</v>
       </c>
       <c r="C33">
-        <v>1805.633333333334</v>
+        <v>6.316666666666666</v>
       </c>
       <c r="D33">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E33">
-        <v>43146.89</v>
+        <v>7199.7</v>
       </c>
       <c r="F33">
-        <v>99.88</v>
+        <v>100</v>
       </c>
       <c r="G33">
-        <v>0.01676528599605523</v>
+        <v>0.01035502958579882</v>
       </c>
       <c r="H33" t="s">
         <v>121</v>
       </c>
       <c r="I33">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1711,25 +1711,25 @@
         <v>98</v>
       </c>
       <c r="C34">
-        <v>1602.3</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="D34">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E34">
-        <v>43149.93</v>
+        <v>7199.87</v>
       </c>
       <c r="F34">
-        <v>99.88</v>
+        <v>100</v>
       </c>
       <c r="G34">
-        <v>0.01577909270216963</v>
+        <v>0.003944773175542407</v>
       </c>
       <c r="H34" t="s">
         <v>121</v>
       </c>
       <c r="I34">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1737,28 +1737,28 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C35">
-        <v>500.293384552002</v>
+        <v>2.75</v>
       </c>
       <c r="D35">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E35">
-        <v>43154.52</v>
+        <v>7199.93</v>
       </c>
       <c r="F35">
-        <v>99.89</v>
+        <v>100</v>
       </c>
       <c r="G35">
-        <v>0.005424063116370809</v>
+        <v>0.01923076923076923</v>
       </c>
       <c r="H35" t="s">
         <v>121</v>
       </c>
       <c r="I35">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1766,28 +1766,28 @@
         <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36">
-        <v>421.7042249043782</v>
+        <v>0.5499999999999999</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="E36">
-        <v>43178.91</v>
+        <v>7199.99</v>
       </c>
       <c r="F36">
-        <v>99.95</v>
+        <v>100</v>
       </c>
       <c r="G36">
-        <v>0.009861932938856016</v>
+        <v>0.02317554240631164</v>
       </c>
       <c r="H36" t="s">
         <v>121</v>
       </c>
       <c r="I36">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1795,28 +1795,28 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37">
-        <v>475.6953704833984</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="E37">
-        <v>43179.32</v>
+        <v>7200</v>
       </c>
       <c r="F37">
-        <v>99.95</v>
+        <v>100</v>
       </c>
       <c r="G37">
-        <v>0.01134122287968442</v>
+        <v>0.02169625246548323</v>
       </c>
       <c r="H37" t="s">
         <v>121</v>
       </c>
       <c r="I37">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1824,28 +1824,28 @@
         <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38">
-        <v>407.5114837646485</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="E38">
-        <v>43183.02</v>
+        <v>7200</v>
       </c>
       <c r="F38">
-        <v>99.95999999999999</v>
+        <v>100</v>
       </c>
       <c r="G38">
-        <v>0.01183431952662722</v>
+        <v>0.02317554240631164</v>
       </c>
       <c r="H38" t="s">
         <v>121</v>
       </c>
       <c r="I38">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1853,28 +1853,28 @@
         <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39">
-        <v>407.5114837646485</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E39">
-        <v>43183.02</v>
+        <v>7200</v>
       </c>
       <c r="F39">
-        <v>99.95999999999999</v>
+        <v>100</v>
       </c>
       <c r="G39">
-        <v>0.01183431952662722</v>
+        <v>0.02218934911242603</v>
       </c>
       <c r="H39" t="s">
         <v>121</v>
       </c>
       <c r="I39">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1882,28 +1882,28 @@
         <v>48</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C40">
-        <v>203.2333333333333</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E40">
-        <v>43191.16</v>
+        <v>7200</v>
       </c>
       <c r="F40">
-        <v>99.98</v>
+        <v>100</v>
       </c>
       <c r="G40">
-        <v>0.01134122287968442</v>
+        <v>0.02218934911242603</v>
       </c>
       <c r="H40" t="s">
         <v>121</v>
       </c>
       <c r="I40">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1911,28 +1911,28 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C41">
-        <v>189.7347195943196</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E41">
-        <v>43194.42</v>
+        <v>7200</v>
       </c>
       <c r="F41">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G41">
-        <v>0.01676528599605523</v>
+        <v>0.02120315581854043</v>
       </c>
       <c r="H41" t="s">
         <v>121</v>
       </c>
       <c r="I41">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1940,19 +1940,19 @@
         <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C42">
-        <v>156.7333333333333</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>32</v>
       </c>
       <c r="E42">
-        <v>43195.1</v>
+        <v>7200</v>
       </c>
       <c r="F42">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G42">
         <v>0.01577909270216963</v>
@@ -1961,7 +1961,7 @@
         <v>121</v>
       </c>
       <c r="I42">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1969,28 +1969,28 @@
         <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C43">
-        <v>89.71666666666667</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E43">
-        <v>43195.73</v>
+        <v>7200</v>
       </c>
       <c r="F43">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G43">
-        <v>0.01035502958579882</v>
+        <v>0.01972386587771203</v>
       </c>
       <c r="H43" t="s">
         <v>121</v>
       </c>
       <c r="I43">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1998,28 +1998,28 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C44">
-        <v>122.6666666666667</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E44">
-        <v>43196.17</v>
+        <v>7200</v>
       </c>
       <c r="F44">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G44">
-        <v>0.01577909270216963</v>
+        <v>0.006903353057199211</v>
       </c>
       <c r="H44" t="s">
         <v>121</v>
       </c>
       <c r="I44">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2027,28 +2027,28 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C45">
-        <v>148.6333333333334</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="E45">
-        <v>43196.54</v>
+        <v>7200</v>
       </c>
       <c r="F45">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G45">
-        <v>0.02120315581854043</v>
+        <v>0.004930966469428008</v>
       </c>
       <c r="H45" t="s">
         <v>121</v>
       </c>
       <c r="I45">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2056,28 +2056,28 @@
         <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C46">
-        <v>84.75</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E46">
-        <v>43196.86</v>
+        <v>7200</v>
       </c>
       <c r="F46">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G46">
-        <v>0.01331360946745562</v>
+        <v>0.003944773175542407</v>
       </c>
       <c r="H46" t="s">
         <v>121</v>
       </c>
       <c r="I46">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2085,28 +2085,28 @@
         <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C47">
-        <v>21.78333333333333</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E47">
-        <v>43197.28</v>
+        <v>7200</v>
       </c>
       <c r="F47">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G47">
-        <v>0.003944773175542407</v>
+        <v>0.005424063116370809</v>
       </c>
       <c r="H47" t="s">
         <v>121</v>
       </c>
       <c r="I47">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2114,28 +2114,28 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C48">
-        <v>113.1789182027181</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="E48">
-        <v>43197.59</v>
+        <v>7200</v>
       </c>
       <c r="F48">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G48">
-        <v>0.02317554240631164</v>
+        <v>0.01134122287968442</v>
       </c>
       <c r="H48" t="s">
         <v>121</v>
       </c>
       <c r="I48">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2143,28 +2143,28 @@
         <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C49">
-        <v>85.56666666666666</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E49">
-        <v>43197.75</v>
+        <v>7200</v>
       </c>
       <c r="F49">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="G49">
-        <v>0.01873767258382643</v>
+        <v>0.01134122287968442</v>
       </c>
       <c r="H49" t="s">
         <v>121</v>
       </c>
       <c r="I49">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2172,28 +2172,28 @@
         <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C50">
-        <v>64.36666666666666</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E50">
-        <v>43198.35</v>
+        <v>7200</v>
       </c>
       <c r="F50">
         <v>100</v>
       </c>
       <c r="G50">
-        <v>0.01923076923076923</v>
+        <v>0.02021696252465483</v>
       </c>
       <c r="H50" t="s">
         <v>121</v>
       </c>
       <c r="I50">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2201,16 +2201,16 @@
         <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C51">
-        <v>18.55</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>27</v>
       </c>
       <c r="E51">
-        <v>43199.31</v>
+        <v>7200</v>
       </c>
       <c r="F51">
         <v>100</v>
@@ -2222,7 +2222,7 @@
         <v>121</v>
       </c>
       <c r="I51">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2230,28 +2230,28 @@
         <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C52">
-        <v>56.15618591308595</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="E52">
-        <v>43199.45</v>
+        <v>7200</v>
       </c>
       <c r="F52">
         <v>100</v>
       </c>
       <c r="G52">
-        <v>0.05029585798816568</v>
+        <v>0.01577909270216963</v>
       </c>
       <c r="H52" t="s">
         <v>121</v>
       </c>
       <c r="I52">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2259,28 +2259,28 @@
         <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C53">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E53">
-        <v>43199.89</v>
+        <v>7200</v>
       </c>
       <c r="F53">
         <v>100</v>
       </c>
       <c r="G53">
-        <v>0.02021696252465483</v>
+        <v>0.01479289940828402</v>
       </c>
       <c r="H53" t="s">
         <v>121</v>
       </c>
       <c r="I53">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2288,28 +2288,28 @@
         <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C54">
-        <v>2.133333333333333</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E54">
-        <v>43199.95</v>
+        <v>7200</v>
       </c>
       <c r="F54">
         <v>100</v>
       </c>
       <c r="G54">
-        <v>0.01972386587771203</v>
+        <v>0.01676528599605523</v>
       </c>
       <c r="H54" t="s">
         <v>121</v>
       </c>
       <c r="I54">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2317,28 +2317,28 @@
         <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E55">
-        <v>43200</v>
+        <v>7200</v>
       </c>
       <c r="F55">
         <v>100</v>
       </c>
       <c r="G55">
-        <v>0.02317554240631164</v>
+        <v>0.01676528599605523</v>
       </c>
       <c r="H55" t="s">
         <v>121</v>
       </c>
       <c r="I55">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2346,28 +2346,28 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E56">
-        <v>43200</v>
+        <v>7200</v>
       </c>
       <c r="F56">
         <v>100</v>
       </c>
       <c r="G56">
-        <v>0.02169625246548323</v>
+        <v>0.01577909270216963</v>
       </c>
       <c r="H56" t="s">
         <v>121</v>
       </c>
       <c r="I56">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2375,28 +2375,28 @@
         <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E57">
-        <v>43200</v>
+        <v>7200</v>
       </c>
       <c r="F57">
         <v>100</v>
       </c>
       <c r="G57">
-        <v>0.007396449704142011</v>
+        <v>0.01577909270216963</v>
       </c>
       <c r="H57" t="s">
         <v>121</v>
       </c>
       <c r="I57">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2404,28 +2404,28 @@
         <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E58">
-        <v>43200</v>
+        <v>7200</v>
       </c>
       <c r="F58">
         <v>100</v>
       </c>
       <c r="G58">
-        <v>0.01577909270216963</v>
+        <v>0.007396449704142011</v>
       </c>
       <c r="H58" t="s">
         <v>121</v>
       </c>
       <c r="I58">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2433,28 +2433,28 @@
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="E59">
-        <v>43200</v>
+        <v>7200</v>
       </c>
       <c r="F59">
         <v>100</v>
       </c>
       <c r="G59">
-        <v>0.003944773175542407</v>
+        <v>0.05029585798816568</v>
       </c>
       <c r="H59" t="s">
         <v>121</v>
       </c>
       <c r="I59">
-        <v>43200</v>
+        <v>7200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>